<commit_message>
Remove Dropix from offered autopilots.
</commit_message>
<xml_diff>
--- a/DDC BOM.xlsx
+++ b/DDC BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UGCS\dd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\github_ddc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F779D1-B1DE-416B-B8A8-DB2CB512C706}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8863372F-1B9D-475F-8A68-C7B0CF00128B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="1800" windowWidth="25455" windowHeight="14115" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="104">
   <si>
     <t>Amount of Drones</t>
   </si>
@@ -284,9 +284,6 @@
     <t>Pixhawk 2.1</t>
   </si>
   <si>
-    <t>Dropix</t>
-  </si>
-  <si>
     <t>Options</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
   </si>
   <si>
     <t>https://store.drotek.com/sirius-rtk-gnss-base-m8p</t>
-  </si>
-  <si>
-    <t>https://store.drotek.com/dropix-autopilot</t>
   </si>
   <si>
     <t>https://eu.mouser.com/ProductDetail/Hirose-Connector/DF13A-6P-125H21?qs=sGAEpiMZZMs%252BGHln7q6pm7BjqI3J1T15bCHcXI1lcLQ%3D</t>
@@ -1012,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1077,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1095,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>7</v>
@@ -1147,7 +1141,7 @@
         <v>80</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" s="20">
         <f>Total!$B$1</f>
@@ -1174,7 +1168,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="20">
         <f>Total!$B$1</f>
@@ -1198,7 +1192,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="20">
@@ -1206,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" s="26">
         <v>5.9</v>
@@ -1221,7 +1215,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="20">
@@ -1229,7 +1223,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F6" s="26">
         <v>54.95</v>
@@ -1267,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="20">
@@ -1275,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="26">
         <v>29.9</v>
@@ -1307,7 +1301,7 @@
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>List!$A$1:$A$2</xm:f>
@@ -1319,7 +1313,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
-            <xm:f>List!$A$4:$A$5</xm:f>
+            <xm:f>List!$A$4:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
@@ -1353,7 +1347,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>7</v>
@@ -1381,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" s="7">
         <v>34.9</v>
@@ -1396,7 +1390,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2">
@@ -1404,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="9">
         <v>15.02</v>
@@ -1419,7 +1413,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="2">
@@ -1427,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4" s="9">
         <v>16.670000000000002</v>
@@ -1519,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="2">
         <v>299.99</v>
@@ -1537,7 +1531,7 @@
         <v>77</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="20">
         <f>Total!$B$1*1</f>
@@ -1817,7 +1811,7 @@
         <v>0.2</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="3">
         <v>2.02</v>
@@ -1907,7 +1901,7 @@
         <v>0.2</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="3">
         <v>3.15</v>
@@ -2093,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="12">
         <v>0.629</v>
@@ -2174,13 +2168,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
       </c>
       <c r="D10" s="47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" s="11">
         <v>0.54100000000000004</v>
@@ -2289,7 +2283,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="47" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E15" s="11">
         <v>8.6999999999999994E-2</v>
@@ -2362,7 +2356,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,7 +2371,7 @@
         <v>78</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="15">
         <v>239.88</v>
@@ -2388,7 +2382,7 @@
         <v>79</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1">
         <v>300</v>
@@ -2407,15 +2401,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="18">
-        <v>120</v>
-      </c>
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="49"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -2444,7 +2432,7 @@
         <v>77</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="20">
         <v>539.88</v>
@@ -2455,10 +2443,9 @@
     <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{E5294B65-72C9-4EDF-8FF4-36F282B5AA70}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{32277754-5445-4BBC-BBA9-77D765B1E988}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{E5294B65-72C9-4EDF-8FF4-36F282B5AA70}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{32277754-5445-4BBC-BBA9-77D765B1E988}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>